<commit_message>
change to currency data point
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/additional-company-information/additional-company-information.xlsx
+++ b/dataland-framework-toolbox/inputs/additional-company-information/additional-company-information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93447\Documents\Dataland\dataland-framework-toolbox\inputs\additional-company-information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B882F804-F43B-4DDA-A4E3-20D1879BFE0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A264B9-D9A9-44CE-B947-08C6C9F6D9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="2205" windowWidth="23760" windowHeight="12345" xr2:uid="{D658489C-BDD5-489B-9246-491A3359E184}"/>
+    <workbookView xWindow="3308" yWindow="3308" windowWidth="21600" windowHeight="11452" xr2:uid="{D658489C-BDD5-489B-9246-491A3359E184}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
   <si>
     <t>Tooltip</t>
   </si>
@@ -120,9 +120,6 @@
   </si>
   <si>
     <t>Enterprise Value Including Cash</t>
-  </si>
-  <si>
-    <t>Number</t>
   </si>
   <si>
     <t>Currency</t>
@@ -593,26 +590,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA2B2C6A-7A28-460C-9762-93D6A2C6CDBB}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="116.85546875" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.59765625" customWidth="1"/>
+    <col min="2" max="2" width="11.1328125" customWidth="1"/>
+    <col min="3" max="3" width="19.59765625" customWidth="1"/>
+    <col min="4" max="4" width="19.1328125" customWidth="1"/>
+    <col min="5" max="5" width="116.86328125" customWidth="1"/>
+    <col min="6" max="6" width="24.1328125" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1"/>
-    <col min="11" max="12" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="9.86328125" customWidth="1"/>
+    <col min="9" max="9" width="18.1328125" customWidth="1"/>
+    <col min="10" max="10" width="12.73046875" customWidth="1"/>
+    <col min="11" max="12" width="18.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -650,7 +647,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -667,16 +664,16 @@
         <v>21</v>
       </c>
       <c r="F2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>32</v>
-      </c>
       <c r="I2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -693,13 +690,13 @@
         <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -716,10 +713,10 @@
         <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -738,14 +735,12 @@
       <c r="F5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="6"/>
+      <c r="I5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -764,14 +759,12 @@
       <c r="F6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="6"/>
+      <c r="I6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="6" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -790,14 +783,12 @@
       <c r="F7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="6"/>
+      <c r="I7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="6" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -816,11 +807,9 @@
       <c r="F8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="6"/>
+      <c r="I8" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix typo in framework
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/additional-company-information/additional-company-information.xlsx
+++ b/dataland-framework-toolbox/inputs/additional-company-information/additional-company-information.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93447\Documents\Dataland\dataland-framework-toolbox\inputs\additional-company-information\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93401\Projects\Dataland\dataland-framework-toolbox\inputs\additional-company-information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A264B9-D9A9-44CE-B947-08C6C9F6D9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5EEAA3-5D1D-4B55-BF8F-375ECA04C29A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3308" yWindow="3308" windowWidth="21600" windowHeight="11452" xr2:uid="{D658489C-BDD5-489B-9246-491A3359E184}"/>
+    <workbookView xWindow="57480" yWindow="-180" windowWidth="29040" windowHeight="15720" xr2:uid="{D658489C-BDD5-489B-9246-491A3359E184}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -95,9 +95,6 @@
     <t>Debt</t>
   </si>
   <si>
-    <t>Balance sheet total</t>
-  </si>
-  <si>
     <t>EVIC</t>
   </si>
   <si>
@@ -138,6 +135,9 @@
   </si>
   <si>
     <t>Report Preupload</t>
+  </si>
+  <si>
+    <t>Balance Sheet Total</t>
   </si>
 </sst>
 </file>
@@ -590,26 +590,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA2B2C6A-7A28-460C-9762-93D6A2C6CDBB}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.59765625" customWidth="1"/>
-    <col min="2" max="2" width="11.1328125" customWidth="1"/>
-    <col min="3" max="3" width="19.59765625" customWidth="1"/>
-    <col min="4" max="4" width="19.1328125" customWidth="1"/>
-    <col min="5" max="5" width="116.86328125" customWidth="1"/>
-    <col min="6" max="6" width="24.1328125" customWidth="1"/>
+    <col min="1" max="1" width="16.6328125" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" customWidth="1"/>
+    <col min="3" max="3" width="19.6328125" customWidth="1"/>
+    <col min="4" max="4" width="19.08984375" customWidth="1"/>
+    <col min="5" max="5" width="116.81640625" customWidth="1"/>
+    <col min="6" max="6" width="24.08984375" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="9.86328125" customWidth="1"/>
-    <col min="9" max="9" width="18.1328125" customWidth="1"/>
-    <col min="10" max="10" width="12.73046875" customWidth="1"/>
-    <col min="11" max="12" width="18.3984375" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" customWidth="1"/>
+    <col min="9" max="9" width="18.08984375" customWidth="1"/>
+    <col min="10" max="10" width="12.7265625" customWidth="1"/>
+    <col min="11" max="12" width="18.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -647,7 +647,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -661,19 +661,19 @@
         <v>14</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>31</v>
-      </c>
       <c r="I2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -687,16 +687,16 @@
         <v>15</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -710,13 +710,13 @@
         <v>16</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -730,17 +730,17 @@
         <v>17</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -754,17 +754,17 @@
         <v>18</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -775,20 +775,20 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -799,17 +799,17 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DALA-5589 Migrate EuTaxonomy Financials To DataPoints (#1073)
Co-authored-by: SiegfriedSobkowiak <71646830+SiegfriedSobkowiak@users.noreply.github.com>
Co-authored-by: Dennis Groh <173401487+dennis-dfine@users.noreply.github.com>
Co-authored-by: StephanWezorke <186339469+StephanWezorke@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/additional-company-information/additional-company-information.xlsx
+++ b/dataland-framework-toolbox/inputs/additional-company-information/additional-company-information.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93401\Projects\Dataland\dataland-framework-toolbox\inputs\additional-company-information\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dataland\dataland\dataland-framework-toolbox\inputs\additional-company-information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5EEAA3-5D1D-4B55-BF8F-375ECA04C29A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8B4E18-2784-4622-8C28-AC865CDBA32A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-180" windowWidth="29040" windowHeight="15720" xr2:uid="{D658489C-BDD5-489B-9246-491A3359E184}"/>
+    <workbookView xWindow="57490" yWindow="-10800" windowWidth="38620" windowHeight="21220" xr2:uid="{D658489C-BDD5-489B-9246-491A3359E184}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -101,9 +101,6 @@
     <t>Does the fiscal year deviate from the calendar year?</t>
   </si>
   <si>
-    <t>The date the fiscal year ends</t>
-  </si>
-  <si>
     <t>Please upload all relevant reports for this dataset in the PDF format.</t>
   </si>
   <si>
@@ -138,6 +135,9 @@
   </si>
   <si>
     <t>Balance Sheet Total</t>
+  </si>
+  <si>
+    <t>The date the fiscal year ends.</t>
   </si>
 </sst>
 </file>
@@ -591,25 +591,25 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" customWidth="1"/>
-    <col min="2" max="2" width="11.08984375" customWidth="1"/>
-    <col min="3" max="3" width="19.6328125" customWidth="1"/>
-    <col min="4" max="4" width="19.08984375" customWidth="1"/>
-    <col min="5" max="5" width="116.81640625" customWidth="1"/>
-    <col min="6" max="6" width="24.08984375" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="116.85546875" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="9.81640625" customWidth="1"/>
-    <col min="9" max="9" width="18.08984375" customWidth="1"/>
-    <col min="10" max="10" width="12.7265625" customWidth="1"/>
-    <col min="11" max="12" width="18.36328125" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="12" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -647,7 +647,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -664,16 +664,16 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>30</v>
-      </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -687,16 +687,16 @@
         <v>15</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -710,13 +710,13 @@
         <v>16</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -730,17 +730,17 @@
         <v>17</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -754,17 +754,17 @@
         <v>18</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -775,20 +775,20 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -802,14 +802,14 @@
         <v>19</v>
       </c>
       <c r="E8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DALA-5898: field names for export
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/additional-company-information/additional-company-information.xlsx
+++ b/dataland-framework-toolbox/inputs/additional-company-information/additional-company-information.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dataland\dataland\dataland-framework-toolbox\inputs\additional-company-information\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93542\Dataland\dataland-framework-toolbox\inputs\additional-company-information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8B4E18-2784-4622-8C28-AC865CDBA32A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7008E2FE-0AD3-40B9-951E-1B00DCA45F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57490" yWindow="-10800" windowWidth="38620" windowHeight="21220" xr2:uid="{D658489C-BDD5-489B-9246-491A3359E184}"/>
+    <workbookView xWindow="57480" yWindow="-9345" windowWidth="29040" windowHeight="15720" xr2:uid="{D658489C-BDD5-489B-9246-491A3359E184}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
   <si>
     <t>Tooltip</t>
   </si>
@@ -138,6 +138,27 @@
   </si>
   <si>
     <t>The date the fiscal year ends.</t>
+  </si>
+  <si>
+    <t>Alias Export</t>
+  </si>
+  <si>
+    <t>FYD</t>
+  </si>
+  <si>
+    <t>FYE</t>
+  </si>
+  <si>
+    <t>RR</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>BST</t>
   </si>
 </sst>
 </file>
@@ -588,28 +609,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA2B2C6A-7A28-460C-9762-93D6A2C6CDBB}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="116.85546875" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" customWidth="1"/>
-    <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1"/>
-    <col min="11" max="12" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" customWidth="1"/>
+    <col min="3" max="3" width="19.54296875" customWidth="1"/>
+    <col min="4" max="5" width="19.1796875" customWidth="1"/>
+    <col min="6" max="6" width="116.81640625" customWidth="1"/>
+    <col min="7" max="7" width="24.1796875" customWidth="1"/>
+    <col min="8" max="8" width="23" customWidth="1"/>
+    <col min="9" max="9" width="9.81640625" customWidth="1"/>
+    <col min="10" max="10" width="18.1796875" customWidth="1"/>
+    <col min="11" max="11" width="12.7265625" customWidth="1"/>
+    <col min="12" max="13" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -622,32 +643,35 @@
       <c r="D1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -660,20 +684,23 @@
       <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -686,17 +713,20 @@
       <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>30</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -709,14 +739,17 @@
       <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -729,18 +762,21 @@
       <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="6"/>
+      <c r="J5" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -753,18 +789,21 @@
       <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="6"/>
+      <c r="J6" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -777,18 +816,21 @@
       <c r="D7" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="6"/>
+      <c r="J7" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -801,14 +843,17 @@
       <c r="D8" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="G8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="6"/>
+      <c r="J8" s="6" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DALA-5788: Adjusted Excel Files for Alias Export
</commit_message>
<xml_diff>
--- a/dataland-framework-toolbox/inputs/additional-company-information/additional-company-information.xlsx
+++ b/dataland-framework-toolbox/inputs/additional-company-information/additional-company-information.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dataland\dataland\dataland-framework-toolbox\inputs\additional-company-information\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d93542\Dataland\dataland-framework-toolbox\inputs\additional-company-information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8B4E18-2784-4622-8C28-AC865CDBA32A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15ED882-7C0C-459A-9EF9-FEB28E8F1A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57490" yWindow="-10800" windowWidth="38620" windowHeight="21220" xr2:uid="{D658489C-BDD5-489B-9246-491A3359E184}"/>
+    <workbookView xWindow="57480" yWindow="-5145" windowWidth="29040" windowHeight="15720" xr2:uid="{D658489C-BDD5-489B-9246-491A3359E184}"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Data Model" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
   <si>
     <t>Tooltip</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>The date the fiscal year ends.</t>
+  </si>
+  <si>
+    <t>Alias Export</t>
   </si>
 </sst>
 </file>
@@ -588,28 +591,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA2B2C6A-7A28-460C-9762-93D6A2C6CDBB}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="116.85546875" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" customWidth="1"/>
-    <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1"/>
-    <col min="11" max="12" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" customWidth="1"/>
+    <col min="3" max="3" width="19.54296875" customWidth="1"/>
+    <col min="4" max="5" width="19.1796875" customWidth="1"/>
+    <col min="6" max="6" width="116.81640625" customWidth="1"/>
+    <col min="7" max="7" width="24.1796875" customWidth="1"/>
+    <col min="8" max="8" width="23" customWidth="1"/>
+    <col min="9" max="9" width="9.81640625" customWidth="1"/>
+    <col min="10" max="10" width="18.1796875" customWidth="1"/>
+    <col min="11" max="11" width="12.7265625" customWidth="1"/>
+    <col min="12" max="13" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -622,32 +625,35 @@
       <c r="D1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -660,20 +666,23 @@
       <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -686,17 +695,20 @@
       <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>30</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -709,14 +721,17 @@
       <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -729,18 +744,21 @@
       <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="6"/>
+      <c r="J5" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -753,18 +771,21 @@
       <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="6"/>
+      <c r="J6" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -777,18 +798,21 @@
       <c r="D7" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="6"/>
+      <c r="J7" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -801,14 +825,17 @@
       <c r="D8" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="G8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="6"/>
+      <c r="J8" s="6" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>